<commit_message>
12 20 story PF alphaM
</commit_message>
<xml_diff>
--- a/Models/LowSeismic 4Floor 12M/Multi/PF alphaM.xlsx
+++ b/Models/LowSeismic 4Floor 12M/Multi/PF alphaM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thesis\Models\LowSeismic 4Floor 12M\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thesis\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DC9ADB-7BEE-4D1F-98B6-5D00184AA091}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6891479E-8422-4076-8A6D-AA452B947B02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="總表" sheetId="1" r:id="rId1"/>
@@ -562,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="6">
-        <f>$C2</f>
+        <f>IF($C2&lt;&gt;"",$C2,"")</f>
         <v>2073.6</v>
       </c>
       <c r="M2" s="9">
@@ -726,7 +726,7 @@
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="6">
-        <f>$C2</f>
+        <f>IF($C2&lt;&gt;"",$C2,"")</f>
         <v>2073.6</v>
       </c>
       <c r="U2" s="9">
@@ -776,7 +776,7 @@
         <v>80.58</v>
       </c>
       <c r="K3" s="6">
-        <f>$C3</f>
+        <f t="shared" ref="K3:K34" si="0">IF($C3&lt;&gt;"",$C3,"")</f>
         <v>518.4</v>
       </c>
       <c r="L3" s="10">
@@ -794,7 +794,7 @@
         <v>-53.2</v>
       </c>
       <c r="S3" s="6">
-        <f>$C3</f>
+        <f t="shared" ref="S3:S34" si="1">IF($C3&lt;&gt;"",$C3,"")</f>
         <v>518.4</v>
       </c>
       <c r="T3" s="10">
@@ -836,7 +836,7 @@
         <v>-14.775</v>
       </c>
       <c r="K4" s="6">
-        <f>$C4</f>
+        <f t="shared" si="0"/>
         <v>518.4</v>
       </c>
       <c r="L4" s="10">
@@ -855,7 +855,7 @@
         <v>85.397999999999996</v>
       </c>
       <c r="S4" s="6">
-        <f>$C4</f>
+        <f t="shared" si="1"/>
         <v>518.4</v>
       </c>
       <c r="T4" s="10">
@@ -894,7 +894,7 @@
         <v>-85.995000000000005</v>
       </c>
       <c r="K5" s="6">
-        <f>$C5</f>
+        <f t="shared" si="0"/>
         <v>518.4</v>
       </c>
       <c r="L5" s="10">
@@ -913,11 +913,11 @@
         <v>10.627000000000001</v>
       </c>
       <c r="S5" s="6">
-        <f>$C5</f>
+        <f t="shared" si="1"/>
         <v>518.4</v>
       </c>
       <c r="T5" s="10">
-        <f t="shared" ref="T5:T6" si="0">R5/$R$3</f>
+        <f t="shared" ref="T5:T6" si="2">R5/$R$3</f>
         <v>-0.19975563909774435</v>
       </c>
       <c r="U5" s="9">
@@ -952,7 +952,7 @@
         <v>-69.358999999999995</v>
       </c>
       <c r="K6" s="6">
-        <f>$C6</f>
+        <f t="shared" si="0"/>
         <v>518.4</v>
       </c>
       <c r="L6" s="10">
@@ -971,11 +971,11 @@
         <v>-93.173000000000002</v>
       </c>
       <c r="S6" s="6">
-        <f>$C6</f>
+        <f t="shared" si="1"/>
         <v>518.4</v>
       </c>
       <c r="T6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7513721804511277</v>
       </c>
       <c r="U6" s="9">
@@ -990,13 +990,287 @@
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C7" s="5"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="R7" s="8"/>
-      <c r="S7" s="5"/>
+      <c r="S7" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="O8" s="8"/>
+      <c r="S8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="W8" s="8"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S13" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S24" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S26" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S27" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S28" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S29" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S30" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S31" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S32" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S33" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S34" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>